<commit_message>
currency statement report updated
</commit_message>
<xml_diff>
--- a/altinkaya_excel_export/export_partner_currency_statement/partner_statement_currency.xlsx
+++ b/altinkaya_excel_export/export_partner_currency_statement/partner_statement_currency.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">CARİ HESAP EKSTRESİ</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">B/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kur</t>
   </si>
   <si>
     <t xml:space="preserve">TL Borç</t>
@@ -285,7 +288,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123840</xdr:rowOff>
     </xdr:from>
@@ -293,7 +296,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>465120</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>579960</xdr:rowOff>
+      <xdr:rowOff>579600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -306,8 +309,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7182360" y="123840"/>
-          <a:ext cx="2561760" cy="456120"/>
+          <a:off x="7185240" y="123840"/>
+          <a:ext cx="2561400" cy="455760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -327,13 +330,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P998"/>
+  <dimension ref="A1:Q998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -342,10 +345,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -366,6 +369,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -383,12 +387,13 @@
       <c r="I2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="7"/>
       <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
@@ -406,6 +411,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -438,24 +444,27 @@
       <c r="J4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="M4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1453,10 +1462,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="G1:N1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="B3:N3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changed currency statement format
</commit_message>
<xml_diff>
--- a/altinkaya_excel_export/export_partner_currency_statement/partner_statement_currency.xlsx
+++ b/altinkaya_excel_export/export_partner_currency_statement/partner_statement_currency.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">CARİ HESAP EKSTRESİ</t>
   </si>
@@ -59,15 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Açıklama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Döviz Borç</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Döviz Alacak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Döviz Bakiye</t>
   </si>
   <si>
     <t xml:space="preserve">B/A</t>
@@ -294,9 +285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
+      <xdr:colOff>464400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>579600</xdr:rowOff>
+      <xdr:rowOff>578880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -309,8 +300,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7185240" y="123840"/>
-          <a:ext cx="2561400" cy="455760"/>
+          <a:off x="7190280" y="123840"/>
+          <a:ext cx="2560680" cy="455040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -333,10 +324,10 @@
   <dimension ref="A1:Q998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -392,8 +383,8 @@
       <c r="L2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
@@ -429,42 +420,36 @@
       <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="K4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="M4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="N4" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>